<commit_message>
adding user input validations
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/notthefinalproject/Competitions Participations.xlsx
+++ b/src/main/java/com/example/notthefinalproject/Competitions Participations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
   <si>
     <t>Competition Name</t>
   </si>
@@ -70,6 +70,9 @@
     <t>SWE</t>
   </si>
   <si>
+    <t>Nawaf Alomari</t>
+  </si>
+  <si>
     <t>Majed Ahmad</t>
   </si>
   <si>
@@ -125,9 +128,6 @@
   </si>
   <si>
     <t>2021-10-02</t>
-  </si>
-  <si>
-    <t>Nawaf Alomari</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -301,22 +301,22 @@
         <v>3.0</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>2.2221926E8</v>
+        <v>2.0193105E8</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -324,22 +324,45 @@
         <v>4.0</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>2.222675E8</v>
+        <v>2.2221926E8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>2.0</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>2.222675E8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="E10" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -367,7 +390,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
@@ -375,7 +398,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -383,7 +406,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
@@ -409,13 +432,13 @@
         <v>2.2225386E8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -426,13 +449,13 @@
         <v>2.2225656E8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -443,13 +466,13 @@
         <v>2.2227926E8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -460,13 +483,13 @@
         <v>2.222567E8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -494,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -502,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -510,7 +533,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
@@ -536,13 +559,13 @@
         <v>2.2225386E8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -553,13 +576,13 @@
         <v>2.2225656E8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -570,13 +593,13 @@
         <v>2.2227926E8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -587,13 +610,13 @@
         <v>2.222567E8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>